<commit_message>
Work in progress celery task not starting
</commit_message>
<xml_diff>
--- a/machine_a/media/processos.xlsx
+++ b/machine_a/media/processos.xlsx
@@ -20,9 +20,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00024273720168180032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00004909620168180062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010586620168180045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00010023320168180045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00004025820168180062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00005228320158180047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00015295020168180088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00008616620168180060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00008608120168180060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000492320178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00009887220168180102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000544520178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00009708020168180060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001627420178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001652920178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00002250220178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001523020178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00001688120178180049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00003936220178180062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00011766520168180102</t>
   </si>
 </sst>
 </file>
@@ -38,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,12 +158,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -123,15 +188,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -141,8 +206,103 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>